<commit_message>
modified:   DANL340/Test4.ipynb new file:   DANL340/va_hrc_alternative.xlsx new file:   DANL340/va_hrc_updated.xlsx new file:   DANL470/Attempt_Hospitals and Doctors Offices 2020 table.csv new file:   DANL470/Attempt_Insured Rates ACS table.csv new file:   DANL470/Attempt_Maternal mortality rates.csv new file:   DANL470/Attempt_Race and Age ACS table.csv modified:   DANL470/Clean_Insured rates.csv modified:   DANL470/Clean_Maternal Mortality Rates.csv modified:   DANL470/Clean_RaceANDAge.csv new file:   DANL470/Origin/Attempt_Hospitals and Doctors Offices 2020 table.xlsx new file:   DANL470/Origin/Attempt_Insured Rates ACS table.xlsx new file:   DANL470/Origin/Attempt_Maternal mortality rates.xlsx new file:   DANL470/Origin/Attempt_Race and Age ACS table.xlsx modified:   DANL470/Origin/Clean_RaceANDAge.xlsx modified:   DANL470/Project1.ipynb new file:   DANL470/Project2.ipynb new file:   DANL470/Project3.ipynb modified:   Lab6/Lab6.ipynb
</commit_message>
<xml_diff>
--- a/DANL470/Origin/Clean_RaceANDAge.xlsx
+++ b/DANL470/Origin/Clean_RaceANDAge.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silen\HealthDataAnalytics\DANL470\Origin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D35AA8-19D1-47A0-B4AF-6E00929B1AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B92FE0-0AEA-46BA-93A1-6D977464BF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1656" windowWidth="19332" windowHeight="10704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RaceANDAge cleanup" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Maryland</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>45 to 54 years</t>
-  </si>
-  <si>
-    <t>RACE</t>
   </si>
   <si>
     <t>Black or African American</t>
@@ -875,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -891,10 +888,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1046,40 +1043,35 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="B11" s="1">
+        <v>331893745</v>
+      </c>
+      <c r="C11" s="1">
+        <v>670050</v>
+      </c>
+      <c r="D11" s="1">
+        <v>6165129</v>
+      </c>
+      <c r="E11" s="1">
+        <v>8642274</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1">
-        <v>331893745</v>
+        <v>40194304</v>
       </c>
       <c r="C12" s="1">
-        <v>670050</v>
+        <v>289302</v>
       </c>
       <c r="D12" s="1">
-        <v>6165129</v>
+        <v>1810345</v>
       </c>
       <c r="E12" s="1">
-        <v>8642274</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1">
-        <v>40194304</v>
-      </c>
-      <c r="C13" s="1">
-        <v>289302</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1810345</v>
-      </c>
-      <c r="E13" s="1">
         <v>1587833</v>
       </c>
     </row>

</xml_diff>